<commit_message>
DESY module loading software
</commit_message>
<xml_diff>
--- a/AdminFolder/Users.xlsx
+++ b/AdminFolder/Users.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA178D0A-CD09-4578-B191-AC1A01D87C6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="12765" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="12765" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Username</t>
   </si>
@@ -28,28 +27,25 @@
     <t>Password</t>
   </si>
   <si>
-    <t>User1</t>
-  </si>
-  <si>
     <t>User2</t>
   </si>
   <si>
     <t>User3</t>
   </si>
   <si>
-    <t>Pass1</t>
-  </si>
-  <si>
     <t>Pass2</t>
   </si>
   <si>
     <t>Pass3</t>
+  </si>
+  <si>
+    <t>desy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -277,7 +273,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -312,7 +308,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -489,18 +485,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,26 +514,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>